<commit_message>
Changed structure, logging and test case setups
Changed resource order
Added test case setup and teardown
Added colorful logging based on failure or pass
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yusuf\Documents\RobotWorks\DataDriven\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC4DF9F-C21A-445B-8C71-98B968B71FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3D7DF9-FEC0-4452-927C-93F103D84D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Navigation_Url</t>
   </si>
@@ -37,9 +37,6 @@
     <t>https://www.google.com</t>
   </si>
   <si>
-    <t>LOG</t>
-  </si>
-  <si>
     <t>https://www.facebook.com</t>
   </si>
   <si>
@@ -49,19 +46,19 @@
     <t>RESULT</t>
   </si>
   <si>
+    <t>https://twitter.com/</t>
+  </si>
+  <si>
+    <t>https://www.nasa.gov/</t>
+  </si>
+  <si>
+    <t>NASA Audiences</t>
+  </si>
+  <si>
     <t>Gmail</t>
   </si>
   <si>
-    <t>https://twitter.com/</t>
-  </si>
-  <si>
-    <t>https://www.nasa.gov/</t>
-  </si>
-  <si>
-    <t>NASA Audiences</t>
-  </si>
-  <si>
-    <t>Join Twitter today.</t>
+    <t>Join Twitter today</t>
   </si>
 </sst>
 </file>
@@ -499,56 +496,48 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>